<commit_message>
sales data from Database, save from mat file to jld file
</commit_message>
<xml_diff>
--- a/Changes from Matlab to Julia.xlsx
+++ b/Changes from Matlab to Julia.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15120" windowHeight="11925" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15120" windowHeight="11925"/>
   </bookViews>
   <sheets>
     <sheet name="Changes from matlab" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="86">
   <si>
     <t>function</t>
   </si>
@@ -242,13 +242,55 @@
   </si>
   <si>
     <t>hcat() and vcat(), when the first variable is any, need to use cat( ,dims=)</t>
+  </si>
+  <si>
+    <t>retrieve from PMT daily data</t>
+  </si>
+  <si>
+    <t>cat multiple variables</t>
+  </si>
+  <si>
+    <t>cat(x…)</t>
+  </si>
+  <si>
+    <t>replace.</t>
+  </si>
+  <si>
+    <t>cannot broadcast</t>
+  </si>
+  <si>
+    <t>map is a quite good tool</t>
+  </si>
+  <si>
+    <t>LinearIndices</t>
+  </si>
+  <si>
+    <t>CartesianIndex</t>
+  </si>
+  <si>
+    <t>transfer</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>Juno.@enter function(inputs)</t>
+  </si>
+  <si>
+    <t>get_country_sizeInfo</t>
+  </si>
+  <si>
+    <t>Sales_rev_turn_raw mat file to jld file</t>
+  </si>
+  <si>
+    <t>salesRevTurnMth mat file to jld file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,13 +298,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Inherit"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -277,11 +330,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,20 +619,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="79.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="59.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -589,7 +646,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -601,7 +658,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -610,7 +667,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -621,7 +678,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -632,7 +689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -643,7 +700,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -654,7 +711,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="B8" t="s">
         <v>16</v>
       </c>
@@ -665,7 +722,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="B9" t="s">
         <v>40</v>
       </c>
@@ -674,6 +731,19 @@
       </c>
       <c r="D9" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="D11" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -683,20 +753,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="79.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -704,7 +774,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -712,7 +782,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -720,7 +790,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -728,7 +798,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -736,7 +806,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -744,22 +814,22 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="B7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="B8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="B9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="B10" t="s">
         <v>36</v>
       </c>
@@ -770,7 +840,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -778,7 +848,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -786,7 +856,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13" t="s">
         <v>56</v>
       </c>
@@ -794,7 +864,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14" t="s">
         <v>60</v>
       </c>
@@ -802,7 +872,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="B15" t="s">
         <v>61</v>
       </c>
@@ -810,7 +880,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" t="s">
         <v>62</v>
       </c>
@@ -818,7 +888,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="B17" t="s">
         <v>65</v>
       </c>
@@ -826,12 +896,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="B18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="B19" t="s">
         <v>69</v>
       </c>
@@ -839,7 +909,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="B20" t="s">
         <v>71</v>
       </c>
@@ -847,100 +917,149 @@
         <v>70</v>
       </c>
     </row>
+    <row r="21" spans="1:3">
+      <c r="B21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="B2" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="F2" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="B4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="B5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="B6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="B7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="B8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="B9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="B10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="B11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="B12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="B13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="B14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="B15" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish 1st industry level code
</commit_message>
<xml_diff>
--- a/Changes from Matlab to Julia.xlsx
+++ b/Changes from Matlab to Julia.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
   <si>
     <t>function</t>
   </si>
@@ -284,6 +284,18 @@
   </si>
   <si>
     <t>salesRevTurnMth mat file to jld file</t>
+  </si>
+  <si>
+    <t>compress = true</t>
+  </si>
+  <si>
+    <t>add_time</t>
+  </si>
+  <si>
+    <t>C:\Users\e0375379\Downloads\DT\Validus_SMECombined\Validus_SMECombined\ProdCode\Industry_Level\ZF_Code\Tools</t>
+  </si>
+  <si>
+    <t>julia trans date type, which is very slow</t>
   </si>
 </sst>
 </file>
@@ -619,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:C18"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -746,6 +758,27 @@
         <v>85</v>
       </c>
     </row>
+    <row r="12" spans="1:4">
+      <c r="D12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -756,7 +789,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>